<commit_message>
Changes done in Classnames
</commit_message>
<xml_diff>
--- a/AdvanceSel/src/test/resources/E18.xlsx
+++ b/AdvanceSel/src/test/resources/E18.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13716" windowHeight="4668" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17016" windowHeight="4572" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DDT" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Contact" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I14"/>
+  <oleSize ref="A1:L14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>